<commit_message>
good shit parece estar funcionando
</commit_message>
<xml_diff>
--- a/Output/Scenario_0.35_3500_0_0_0_0_0_0_fuck_u.xlsx
+++ b/Output/Scenario_0.35_3500_0_0_0_0_0_0_fuck_u.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d97d3de92643fad0/Documents/Documents/Mestrado/PlanejamentoEstocasticoDeRotas/Output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="11_258DEA403018A65302F20A5EA041B45A3CCF5C43" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E8829F8-8297-4C12-915C-A8CFCAE4A98A}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="11_258DEA403018A65302F20A5EA041B45A3CCF5C43" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB848E84-04EF-41FC-8C4E-3CE97A30EA7B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descrição do cenário" sheetId="1" r:id="rId1"/>
@@ -2556,7 +2556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:P201"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -16261,10 +16261,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AA14"/>
+  <dimension ref="A1:AD14"/>
   <sheetViews>
     <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13"/>
+      <selection activeCell="AD11" sqref="AD2:AD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16296,7 +16296,7 @@
     <col min="27" max="27" width="18.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
@@ -16376,7 +16376,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -16458,8 +16458,20 @@
       <c r="AA2" s="2">
         <v>327748.58025</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AB2">
+        <f>15680000/4/8</f>
+        <v>490000</v>
+      </c>
+      <c r="AC2">
+        <f>Z2+Y2+X2+W2+AB2</f>
+        <v>598212.41786460788</v>
+      </c>
+      <c r="AD2">
+        <f>AC2/3500</f>
+        <v>170.91783367560225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -16541,8 +16553,20 @@
       <c r="AA3" s="2">
         <v>993747.10499999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AB3">
+        <f t="shared" ref="AB3:AB11" si="0">15680000/4/8</f>
+        <v>490000</v>
+      </c>
+      <c r="AC3">
+        <f t="shared" ref="AC3:AC11" si="1">Z3+Y3+X3+W3+AB3</f>
+        <v>1387002.7901080349</v>
+      </c>
+      <c r="AD3">
+        <f t="shared" ref="AD3:AD11" si="2">AC3/3500</f>
+        <v>396.28651145943854</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -16624,8 +16648,20 @@
       <c r="AA4" s="2">
         <v>229712.21325</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AB4">
+        <f t="shared" si="0"/>
+        <v>490000</v>
+      </c>
+      <c r="AC4">
+        <f t="shared" si="1"/>
+        <v>895060.62933599413</v>
+      </c>
+      <c r="AD4">
+        <f t="shared" si="2"/>
+        <v>255.73160838171262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -16707,8 +16743,20 @@
       <c r="AA5" s="2">
         <v>168595.245</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AB5">
+        <f t="shared" si="0"/>
+        <v>490000</v>
+      </c>
+      <c r="AC5">
+        <f t="shared" si="1"/>
+        <v>1539296.9090198916</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="2"/>
+        <v>439.79911686282617</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -16790,8 +16838,20 @@
       <c r="AA6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AB6">
+        <f t="shared" si="0"/>
+        <v>490000</v>
+      </c>
+      <c r="AC6">
+        <f t="shared" si="1"/>
+        <v>1268648.4333333333</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="2"/>
+        <v>362.47098095238096</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -16873,8 +16933,20 @@
       <c r="AA7" s="2">
         <v>1179009.1170000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AB7">
+        <f t="shared" si="0"/>
+        <v>490000</v>
+      </c>
+      <c r="AC7">
+        <f t="shared" si="1"/>
+        <v>1443811.3340198917</v>
+      </c>
+      <c r="AD7">
+        <f t="shared" si="2"/>
+        <v>412.51752400568336</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -16956,8 +17028,20 @@
       <c r="AA8" s="2">
         <v>168242.88</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AB8">
+        <f t="shared" si="0"/>
+        <v>490000</v>
+      </c>
+      <c r="AC8">
+        <f t="shared" si="1"/>
+        <v>888523.78628043854</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="2"/>
+        <v>253.86393893726816</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -17039,8 +17123,20 @@
       <c r="AA9" s="2">
         <v>263369.59350000008</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AB9">
+        <f t="shared" si="0"/>
+        <v>490000</v>
+      </c>
+      <c r="AC9">
+        <f t="shared" si="1"/>
+        <v>1353265.6089969238</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="2"/>
+        <v>386.64731685626396</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -17122,8 +17218,20 @@
       <c r="AA10" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AB10">
+        <f t="shared" si="0"/>
+        <v>490000</v>
+      </c>
+      <c r="AC10">
+        <f t="shared" si="1"/>
+        <v>744345.54453127459</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="2"/>
+        <v>212.67015558036417</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -17205,98 +17313,110 @@
       <c r="AA11" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AB11">
+        <f t="shared" si="0"/>
+        <v>490000</v>
+      </c>
+      <c r="AC11">
+        <f t="shared" si="1"/>
+        <v>607110.59333333338</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="2"/>
+        <v>173.46016952380953</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D13" s="2">
-        <f t="shared" ref="D13:AA13" si="0">SUM(D2:D11)</f>
+        <f t="shared" ref="D13:AA13" si="3">SUM(D2:D11)</f>
         <v>130.46272802465882</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6948.2127019999998</v>
       </c>
       <c r="F13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>22.19092509920635</v>
       </c>
       <c r="G13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1781.5</v>
       </c>
       <c r="H13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.7593014219576721</v>
       </c>
       <c r="I13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1781.5</v>
       </c>
       <c r="J13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.7818931878306878</v>
       </c>
       <c r="K13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>234.5</v>
       </c>
       <c r="L13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.23496362433862433</v>
       </c>
       <c r="M13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>234.5</v>
       </c>
       <c r="N13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.19958333333333331</v>
       </c>
       <c r="O13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.9757415674603176</v>
       </c>
       <c r="P13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.333333333333333</v>
       </c>
       <c r="Q13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>28.5</v>
       </c>
       <c r="R13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>8075.5</v>
       </c>
       <c r="S13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.1457757142857146</v>
       </c>
       <c r="T13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>15847262.355</v>
       </c>
       <c r="U13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2890622.5</v>
       </c>
       <c r="V13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>296635</v>
       </c>
       <c r="W13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3777340.2182403905</v>
       </c>
       <c r="X13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>342734.39997222216</v>
       </c>
       <c r="Y13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>139203.4286111111</v>
       </c>
       <c r="Z13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1566000</v>
       </c>
       <c r="AA13" s="2">
@@ -17304,7 +17424,7 @@
         <v>3330424.7340000002</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="Z14" s="2">
         <f>Z13*4</f>
         <v>6264000</v>
@@ -17321,10 +17441,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17345,9 +17465,10 @@
     <col min="14" max="14" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.77734375" customWidth="1"/>
     <col min="17" max="17" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>25</v>
       </c>
@@ -17391,7 +17512,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -17447,8 +17568,12 @@
         <f>N2*1.25</f>
         <v>48710781.471737549</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R2" s="2">
+        <f>L2/3500/4</f>
+        <v>4476.475408099288</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -17504,8 +17629,12 @@
         <f t="shared" ref="Q3:Q13" si="3">N3*1.25</f>
         <v>48653909.688423306</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R3" s="2">
+        <f t="shared" ref="R3:R13" si="4">L3/3500/4</f>
+        <v>4789.0221520527602</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -17561,8 +17690,12 @@
         <f t="shared" si="3"/>
         <v>48640660.915675946</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R4" s="2">
+        <f t="shared" si="4"/>
+        <v>4856.680522467198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -17618,8 +17751,12 @@
         <f t="shared" si="3"/>
         <v>48627853.639983401</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R5" s="2">
+        <f t="shared" si="4"/>
+        <v>4949.3856574990514</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -17675,8 +17812,12 @@
         <f t="shared" si="3"/>
         <v>48623088.442203365</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R6" s="2">
+        <f t="shared" si="4"/>
+        <v>4941.0049020544784</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -17732,8 +17873,12 @@
         <f t="shared" si="3"/>
         <v>48671230.234118626</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R7" s="2">
+        <f t="shared" si="4"/>
+        <v>4643.690651663921</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -17789,8 +17934,12 @@
         <f t="shared" si="3"/>
         <v>48641367.482506409</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R8" s="2">
+        <f t="shared" si="4"/>
+        <v>4835.9123252860809</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -17846,8 +17995,12 @@
         <f t="shared" si="3"/>
         <v>48630313.31568379</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R9" s="2">
+        <f t="shared" si="4"/>
+        <v>4930.2253961819306</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -17903,8 +18056,12 @@
         <f t="shared" si="3"/>
         <v>48758726.400443725</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R10" s="2">
+        <f t="shared" si="4"/>
+        <v>4277.8464999539274</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -17960,8 +18117,12 @@
         <f t="shared" si="3"/>
         <v>48635216.490396008</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R11" s="2">
+        <f t="shared" si="4"/>
+        <v>4908.9737329512009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -18017,8 +18178,12 @@
         <f t="shared" si="3"/>
         <v>48636029.279166833</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R12" s="2">
+        <f t="shared" si="4"/>
+        <v>4796.6227857381045</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -18074,8 +18239,12 @@
         <f t="shared" si="3"/>
         <v>48641931.890963182</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R13" s="2">
+        <f t="shared" si="4"/>
+        <v>4870.2310532693255</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B15" s="2">
         <f>SUM(B2:B13)</f>
         <v>824401949.5999999</v>
@@ -18089,67 +18258,91 @@
         <v>16039030</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" ref="E15:L15" si="4">SUM(E2:E13)</f>
+        <f t="shared" ref="E15:L15" si="5">SUM(E2:E13)</f>
         <v>47472</v>
       </c>
       <c r="F15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75168000</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>170212121.82000002</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>181068531.17170841</v>
       </c>
       <c r="J15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>22700356.22933333</v>
       </c>
       <c r="K15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>188160000</v>
       </c>
       <c r="L15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>801864995.22104168</v>
       </c>
       <c r="M15" s="2">
         <f>SUM(M2:M13)</f>
         <v>22536954.37895827</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O15" s="2">
+        <f>O13*8</f>
+        <v>22236.31172158317</v>
+      </c>
+      <c r="R15" s="2">
+        <f>R13*8</f>
+        <v>38961.848426154604</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="L17" s="2">
+        <f>L5/3500</f>
+        <v>19797.542629996206</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>51</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="L18" s="2">
+        <f>L17/4</f>
+        <v>4949.3856574990514</v>
+      </c>
+      <c r="M18">
+        <f>40000/8</f>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>52</v>
       </c>
       <c r="B19">
         <v>-0.42080011666457517</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="L19" s="2">
+        <f>L6/4</f>
+        <v>17293517.157190673</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -73469,7 +73662,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>